<commit_message>
Roll Back Part -1
</commit_message>
<xml_diff>
--- a/Assets/data/Book_insert.xlsx
+++ b/Assets/data/Book_insert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\LibraryManagement\Assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB9B7BE-AC55-4670-BDA5-963641D1E4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F41242-6030-416E-A125-608D7E61FB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8E09630E-FBB8-4CD5-98D8-40C1A54718B3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E09630E-FBB8-4CD5-98D8-40C1A54718B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,23 +486,23 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="11" max="13" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="11" max="13" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -590,9 +590,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>150</v>
+        <v>1000</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -628,7 +628,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Roll Back Part -2
</commit_message>
<xml_diff>
--- a/Assets/data/Book_insert.xlsx
+++ b/Assets/data/Book_insert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\LibraryManagement\Assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03852CE-ABFD-468B-8D7C-0A2AA44DF41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48153B3B-CA17-4966-A550-2EA98B7E16A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8E09630E-FBB8-4CD5-98D8-40C1A54718B3}"/>
+    <workbookView xWindow="3864" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{8E09630E-FBB8-4CD5-98D8-40C1A54718B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,23 +480,23 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="11" max="13" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="11" max="13" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,9 +540,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>150</v>
+        <v>1000</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -578,7 +578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Student insert buffer roll backed
</commit_message>
<xml_diff>
--- a/Assets/data/Book_insert.xlsx
+++ b/Assets/data/Book_insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\LibraryManagement\Assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02866D8-2981-4B12-ADB5-0EB8B0EEA3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E07101-15DE-4890-B2A4-F78D05AA3807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3864" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{8E09630E-FBB8-4CD5-98D8-40C1A54718B3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E09630E-FBB8-4CD5-98D8-40C1A54718B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,7 +542,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1100</v>
+        <v>1150</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -575,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="N2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>